<commit_message>
[Updated] Process to select center of fibre point
</commit_message>
<xml_diff>
--- a/【Manual】Fibre_mode_fitting_tool.xlsx
+++ b/【Manual】Fibre_mode_fitting_tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fah_temp\Gaussian_fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAFA975-9CA0-4B86-871D-302589031865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9653DA-27C3-455C-9DD5-97E42CCD81A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27A076E-494D-41D2-8CBC-858DE9BFF09C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Overall flowchart</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Fill "Radius", "Sensor pixel" and "Sensor magnification" value, then click "OK"</t>
   </si>
   <si>
-    <t>Tool will show progress bar during execution</t>
-  </si>
-  <si>
     <t>After the tool finishes running, "DONE" will appear in the command window</t>
   </si>
   <si>
@@ -91,6 +88,12 @@
   </si>
   <si>
     <t>Objective : This tool use for fibre mode fitting in 3 methods as below</t>
+  </si>
+  <si>
+    <t>Click to select center of fibre, tool will adjust position and crop again for image that fibre is at the center</t>
+  </si>
+  <si>
+    <t>Start Gaussain fitting and tool will show progress bar during execution</t>
   </si>
 </sst>
 </file>
@@ -167,21 +170,388 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Graphic 8" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D96A81-71F3-4B8B-BB61-360F164DBC78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="238125"/>
+          <a:ext cx="238125" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62316BF5-7200-4102-BB11-FD93B35344A0}"/>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E6B4CA1-FC35-90CB-2B64-A3CC71AD3AA5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="1466850"/>
+          <a:ext cx="8191500" cy="10477500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Graphic 7" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1428DDC9-7A40-4762-B4F9-33D98A68008E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="1962150"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Graphic 9" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C127399-3083-4C36-5D48-2897E575A30F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="3009900"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Graphic 11" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{137CE656-A702-F34B-502F-8D11D13E34A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="4343400"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Graphic 12" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E1E3115-256A-FD36-F0A4-55BC1E38FD55}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="847725" y="5010150"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Graphic 13" descr="User with solid fill">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3EFA01B-9977-4751-8277-F3E21E7D9048}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="838200" y="6696075"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476572</xdr:colOff>
+      <xdr:row>147</xdr:row>
+      <xdr:rowOff>57381</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2317E3D-A1EB-FF1A-C1F4-A255C3376FA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -197,8 +567,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="609600" y="381000"/>
-          <a:ext cx="8191500" cy="9239250"/>
+          <a:off x="266700" y="26450925"/>
+          <a:ext cx="2305372" cy="1657581"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -210,22 +580,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>97346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114885</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>68771</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Graphic 2" descr="User with solid fill">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{733D5838-4633-4AE7-9D1A-64D419018D9F}"/>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FC0D1EC-2DB4-2398-E45C-30B0398D3DE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -234,24 +604,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1200150" y="866775"/>
-          <a:ext cx="371475" cy="371475"/>
+          <a:off x="266700" y="19385471"/>
+          <a:ext cx="4382085" cy="3781425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -263,22 +624,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>76551</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38305</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Graphic 3" descr="User with solid fill">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8D44DCF-152E-4BEF-B3E9-C8BF054FC9A6}"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA62197-95D3-1CC7-5E44-763D87C43AFF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -287,224 +648,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1200150" y="2200275"/>
-          <a:ext cx="371475" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Graphic 4" descr="User with solid fill">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56D6D51B-BA96-45FF-8070-ECED37088D84}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1200150" y="3895725"/>
-          <a:ext cx="371475" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Graphic 5" descr="User with solid fill">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8C9048F-2D0D-421C-8C7C-DDAF12F65D9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5191125" y="5372100"/>
-          <a:ext cx="371475" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Graphic 8" descr="User with solid fill">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71D96A81-71F3-4B8B-BB61-360F164DBC78}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
-              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId3"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="257175" y="238125"/>
-          <a:ext cx="238125" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>76551</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38305</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA62197-95D3-1CC7-5E44-763D87C43AFF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -830,7 +974,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -874,7 +1018,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -978,7 +1122,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1281,7 +1425,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1635,13 +1779,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114826</xdr:colOff>
-      <xdr:row>89</xdr:row>
+      <xdr:row>98</xdr:row>
       <xdr:rowOff>66858</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1658,7 +1802,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1679,13 +1823,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>87</xdr:row>
+      <xdr:row>96</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1744,7 +1888,7 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>86</xdr:row>
+      <xdr:row>95</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3014095" cy="264560"/>
@@ -1810,62 +1954,18 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19904</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>10262</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="Picture 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E10DE8C9-93D7-5B6F-B5C2-A70AC7E08F8C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="17449800"/>
-          <a:ext cx="6115904" cy="5277587"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>103</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1880,8 +1980,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3409950" y="19678650"/>
-          <a:ext cx="247650" cy="257175"/>
+          <a:off x="3076575" y="20916901"/>
+          <a:ext cx="228600" cy="228600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1922,23 +2022,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>286881</xdr:colOff>
-      <xdr:row>119</xdr:row>
-      <xdr:rowOff>10262</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>181426</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>19219</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="30" name="Picture 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8A4DEDC-CBB1-088B-AFE6-71ACEF2FA34D}"/>
+        <xdr:cNvPr id="36" name="Picture 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C24E1C-5180-BCC2-B932-CA2821230A5D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1947,15 +2047,15 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7077075" y="17449800"/>
-          <a:ext cx="8106906" cy="5277587"/>
+          <a:off x="266700" y="24003000"/>
+          <a:ext cx="3229426" cy="1209844"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1964,25 +2064,74 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>71435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247940</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>109726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A12282-E09B-CC60-D605-E77B9ADB70BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3314700" y="27741560"/>
+          <a:ext cx="2076740" cy="1371791"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>104</xdr:row>
-      <xdr:rowOff>109906</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>157531</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Arrow: Right 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3014ADAB-C34C-4A2F-964A-23ECA04AF657}"/>
+        <xdr:cNvPr id="40" name="Rectangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E58521-3B5C-4C4E-9306-9C40B3E301BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1990,12 +2139,18 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6591300" y="19969531"/>
-          <a:ext cx="333375" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
+          <a:off x="285750" y="26841451"/>
+          <a:ext cx="2209800" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -2026,432 +2181,82 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>28574</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="Speech Bubble: Rectangle 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5748414D-B361-B5BA-CE38-50B11970AB2B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12706349" y="21297900"/>
-          <a:ext cx="2219325" cy="409575"/>
-        </a:xfrm>
-        <a:prstGeom prst="wedgeRectCallout">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -3339"/>
-            <a:gd name="adj2" fmla="val -112962"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF00"/>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>You</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> can select again by click "Yes"</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>121</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>514592</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>47802</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="33" name="Picture 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B42E760E-62FE-1862-8601-6CBEA1ABBBAA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="23212425"/>
-          <a:ext cx="1733792" cy="1267002"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>514592</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>171607</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FF7D680-DBA9-687F-6DE8-1A6754C46E4C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2705100" y="23288625"/>
-          <a:ext cx="1733792" cy="1124107"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>152677</xdr:colOff>
-      <xdr:row>127</xdr:row>
-      <xdr:rowOff>171607</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="35" name="Picture 34">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{17A80B45-3D2F-C5F1-E2AF-4DFE89981AC8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5143500" y="23288625"/>
-          <a:ext cx="1981477" cy="1124107"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>181426</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>19219</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="36" name="Picture 35">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C24E1C-5180-BCC2-B932-CA2821230A5D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="25146000"/>
-          <a:ext cx="3229426" cy="1209844"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47972</xdr:colOff>
-      <xdr:row>153</xdr:row>
-      <xdr:rowOff>57381</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CC45E40-76A0-9DE4-7B95-85BA3DCD1999}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="26831925"/>
-          <a:ext cx="2486372" cy="1657581"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>71435</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247940</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>109726</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A12282-E09B-CC60-D605-E77B9ADB70BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3314700" y="27741560"/>
-          <a:ext cx="2076740" cy="1371791"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>185831</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="42" name="Straight Arrow Connector 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F47C1B-91CA-449C-A1A9-82D0B06502F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="40" idx="3"/>
+          <a:endCxn id="38" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2495550" y="26955751"/>
+          <a:ext cx="819150" cy="709705"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
           <a:solidFill>
             <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
+          <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>139</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>140</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>505290</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>76385</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="39" name="Picture 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5B2091-559C-1F12-168F-333FFC934DCA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5972175" y="26803350"/>
-          <a:ext cx="3334215" cy="1324160"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>144</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Rectangle 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57E58521-3B5C-4C4E-9306-9C40B3E301BD}"/>
+        <xdr:cNvPr id="43" name="Rectangle 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF1AFDA2-BF72-4529-B04C-CDDD930ACA9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2459,8 +2264,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="285750" y="26841451"/>
-          <a:ext cx="2209800" cy="228600"/>
+          <a:off x="3333750" y="27755851"/>
+          <a:ext cx="1990725" cy="209549"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2501,35 +2306,36 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>185831</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>166777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>140</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="42" name="Straight Arrow Connector 41">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57F47C1B-91CA-449C-A1A9-82D0B06502F4}"/>
+        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FDD59A7-64AE-434B-BE5C-3E61D2641C30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="40" idx="3"/>
-          <a:endCxn id="38" idx="1"/>
+          <a:cxnSpLocks/>
+          <a:stCxn id="43" idx="3"/>
+          <a:endCxn id="56" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2495550" y="26955751"/>
-          <a:ext cx="819150" cy="709705"/>
+        <a:xfrm flipV="1">
+          <a:off x="5324475" y="26312902"/>
+          <a:ext cx="657225" cy="404724"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2562,21 +2368,21 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>145</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:row>143</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="Rectangle 42">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF1AFDA2-BF72-4529-B04C-CDDD930ACA9D}"/>
+        <xdr:cNvPr id="52" name="Rectangle 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0612BC4B-F7E7-53A9-C92D-4E5C2A63A688}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2584,7 +2390,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3333750" y="27755851"/>
+          <a:off x="3333750" y="28565476"/>
           <a:ext cx="1990725" cy="209549"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2626,131 +2432,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>145</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>176305</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>146</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="44" name="Straight Arrow Connector 43">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FDD59A7-64AE-434B-BE5C-3E61D2641C30}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="43" idx="3"/>
-          <a:endCxn id="39" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5324475" y="27465430"/>
-          <a:ext cx="647700" cy="395196"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>141</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>158</xdr:row>
-      <xdr:rowOff>97491</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{055E342D-7C50-59A7-98E4-6D87EC5003E1}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9801225" y="27070050"/>
-          <a:ext cx="3114675" cy="3174066"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>149</xdr:row>
-      <xdr:rowOff>133351</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="52" name="Rectangle 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0612BC4B-F7E7-53A9-C92D-4E5C2A63A688}"/>
+        <xdr:cNvPr id="53" name="Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9117AADF-1638-DF24-B5E0-275BFAAE7CF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2758,7 +2456,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3333750" y="28565476"/>
+          <a:off x="3333750" y="28832176"/>
           <a:ext cx="1990725" cy="209549"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2800,81 +2498,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>151</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="Rectangle 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9117AADF-1638-DF24-B5E0-275BFAAE7CF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3333750" y="28832176"/>
-          <a:ext cx="1990725" cy="209549"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>150</xdr:row>
-      <xdr:rowOff>34458</xdr:rowOff>
+      <xdr:row>144</xdr:row>
+      <xdr:rowOff>33909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>144</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2887,14 +2519,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="52" idx="3"/>
-          <a:endCxn id="47" idx="1"/>
+          <a:endCxn id="59" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5324475" y="28657083"/>
-          <a:ext cx="4476750" cy="13168"/>
+          <a:off x="5324475" y="27513534"/>
+          <a:ext cx="4486275" cy="13717"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2923,67 +2556,18 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>500409</xdr:colOff>
-      <xdr:row>154</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>190673</xdr:colOff>
-      <xdr:row>167</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="58" name="Picture 57">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C43C8EAF-8C42-3CDF-D1F8-C8BCFA4063E6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3205509" y="29451300"/>
-          <a:ext cx="6395864" cy="2486025"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>145</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>40741</xdr:colOff>
-      <xdr:row>154</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:colOff>38304</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2995,14 +2579,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
+          <a:cxnSpLocks/>
           <a:stCxn id="53" idx="3"/>
-          <a:endCxn id="58" idx="0"/>
+          <a:endCxn id="61" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5324475" y="28936951"/>
-          <a:ext cx="1078966" cy="514349"/>
+          <a:off x="5324475" y="27793951"/>
+          <a:ext cx="1076529" cy="504824"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3035,13 +2620,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>143</xdr:row>
+      <xdr:row>137</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3120,6 +2705,623 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1733792" cy="1124107"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3805CF2-9E50-4B21-9E1D-FDB7EAB6B0EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2705100" y="25003125"/>
+          <a:ext cx="1733792" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1981477" cy="1124107"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ECE067-1CE8-4876-8283-1FA4E281EFB6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5143500" y="25003125"/>
+          <a:ext cx="1981477" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514592</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>171607</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7ED2A0-AA36-AE2B-1E8F-A6BE8CEEA72A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="15859125"/>
+          <a:ext cx="1733792" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102348</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>222089</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>70866</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E3494D8-2F4E-AFE6-2A30-6AE99C8B15E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245848" y="19383375"/>
+          <a:ext cx="4386941" cy="3785616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>329292</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>70866</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4D728B-554B-0458-41F1-CA0E38277F8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10229851" y="19383375"/>
+          <a:ext cx="4386941" cy="3785616"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>246729</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>154496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>580104</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>11621</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="48" name="Arrow: Right 47">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57AC2900-8F25-48BD-A286-03682E16104A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4780629" y="21157121"/>
+          <a:ext cx="333375" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>353933</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>154496</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>77708</xdr:colOff>
+      <xdr:row>113</xdr:row>
+      <xdr:rowOff>11621</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="49" name="Arrow: Right 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C63D36B-228D-2652-29F2-227F712426DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9764633" y="21157121"/>
+          <a:ext cx="333375" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>180976</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>219076</xdr:colOff>
+      <xdr:row>121</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="50" name="Speech Bubble: Rectangle 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4926FAF2-3D0E-5403-7554-70448139DF79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13592176" y="22517101"/>
+          <a:ext cx="2133600" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -40886"/>
+            <a:gd name="adj2" fmla="val -83261"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFF00"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>You can click "Yes" to select again</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4283480" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="TextBox 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{881137C3-3333-4F61-AD83-18C9513F8F5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10287000" y="19307175"/>
+          <a:ext cx="4283480" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Tool will adjust position and crop again for image that fibre is at the center</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>524342</xdr:colOff>
+      <xdr:row>141</xdr:row>
+      <xdr:rowOff>47804</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C407BF7B-B12F-94B7-5C1F-CB743249D1C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5981700" y="25669875"/>
+          <a:ext cx="3343742" cy="1286054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>135</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>453202</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>96393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED12F2A-AC04-60AB-065F-442A35C8B425}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9810750" y="25927050"/>
+          <a:ext cx="3101152" cy="3172968"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>200433</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>67818</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE762BC-479B-EA7D-B342-752A5E1844F4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3190875" y="28298775"/>
+          <a:ext cx="6420258" cy="2487168"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3458,25 +3660,25 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -3501,7 +3703,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B5091E-4ABE-4EB2-95DD-AC45409874BA}">
-  <dimension ref="A1:B140"/>
+  <dimension ref="A1:B134"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3552,7 +3754,7 @@
         <v>5</v>
       </c>
       <c r="B82" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -3560,36 +3762,41 @@
         <v>6</v>
       </c>
       <c r="B91" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>7</v>
+      </c>
+      <c r="B100" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121">
-        <v>7</v>
-      </c>
-      <c r="B121" t="s">
-        <v>10</v>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124">
         <v>8</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B131" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
         <v>9</v>
       </c>
-      <c r="B140" t="s">
-        <v>13</v>
+      <c r="B134" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Updated] Added browse button for fit file
</commit_message>
<xml_diff>
--- a/【Manual】Fibre_mode_fitting_tool.xlsx
+++ b/【Manual】Fibre_mode_fitting_tool.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\fah_temp\Gaussian_fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9653DA-27C3-455C-9DD5-97E42CCD81A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65035D76-DFD2-49B5-B404-CB908ED19D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A27A076E-494D-41D2-8CBC-858DE9BFF09C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Overall flowchart</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Manual</t>
   </si>
   <si>
-    <t>Tool and target fit file MUST be located in same location</t>
-  </si>
-  <si>
     <t>Open tool folder in Visual Studio Code</t>
   </si>
   <si>
@@ -61,9 +58,6 @@
   </si>
   <si>
     <t>Click "Run Python File" button</t>
-  </si>
-  <si>
-    <t>Fill target fit file path, then click "OK"</t>
   </si>
   <si>
     <t>Select region of interest by drag left mouse</t>
@@ -94,6 +88,9 @@
   </si>
   <si>
     <t>Start Gaussain fitting and tool will show progress bar during execution</t>
+  </si>
+  <si>
+    <t>Browse target fit file path, then click "OK"</t>
   </si>
 </sst>
 </file>
@@ -537,21 +534,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>476572</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>57381</xdr:rowOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>67280</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>133543</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="55" name="Picture 54">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2317E3D-A1EB-FF1A-C1F4-A255C3376FA4}"/>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7DEE5E10-1EB2-BC0F-0987-92FEAE07BB86}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -567,8 +564,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="26450925"/>
-          <a:ext cx="2305372" cy="1657581"/>
+          <a:off x="266700" y="15563850"/>
+          <a:ext cx="4334480" cy="1381318"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,21 +578,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>97346</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114885</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>68771</xdr:rowOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>476572</xdr:colOff>
+      <xdr:row>137</xdr:row>
+      <xdr:rowOff>57381</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="41" name="Picture 40">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FC0D1EC-2DB4-2398-E45C-30B0398D3DE7}"/>
+        <xdr:cNvPr id="55" name="Picture 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2317E3D-A1EB-FF1A-C1F4-A255C3376FA4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -611,8 +608,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="19385471"/>
-          <a:ext cx="4382085" cy="3781425"/>
+          <a:off x="266700" y="26450925"/>
+          <a:ext cx="2305372" cy="1657581"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -625,21 +622,21 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>76551</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38305</xdr:rowOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>97346</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>114885</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>68771</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAA62197-95D3-1CC7-5E44-763D87C43AFF}"/>
+        <xdr:cNvPr id="41" name="Picture 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FC0D1EC-2DB4-2398-E45C-30B0398D3DE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -655,8 +652,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="523875"/>
-          <a:ext cx="2514951" cy="1467055"/>
+          <a:off x="266700" y="19385471"/>
+          <a:ext cx="4382085" cy="3781425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -665,25 +662,113 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>295742</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152747</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CA4FE9-8671-EC29-EF42-231244A49FC5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="2667000"/>
+          <a:ext cx="3343742" cy="2486372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>591092</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9968</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90662B2-DED9-80E6-BD38-4D0D997612BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="2409825"/>
+          <a:ext cx="3886742" cy="3172268"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5868B824-F9BD-DF39-5ED3-0F0281C83F87}"/>
+        <xdr:cNvPr id="10" name="Arrow: Right 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{648F1480-C9C4-0517-5FA9-B2B4316172AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -691,18 +776,12 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314325" y="581025"/>
-          <a:ext cx="2324100" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
+          <a:off x="3829050" y="4371975"/>
+          <a:ext cx="333375" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -731,25 +810,69 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>544447</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>86391</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4843C52-C2B9-BF1F-F744-06C88DA58DFD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="6029325"/>
+          <a:ext cx="10907647" cy="4772691"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="Rectangle 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52CC87B2-B65C-96F6-F533-96806C7EFA6A}"/>
+        <xdr:cNvPr id="12" name="Rectangle 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E64B640A-9FE7-47F0-90BB-E3A2667A15E1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -757,8 +880,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="314325" y="857250"/>
-          <a:ext cx="2324100" cy="1047750"/>
+          <a:off x="571500" y="2724150"/>
+          <a:ext cx="323850" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -797,263 +920,25 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="674224" cy="266098"/>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A0E8C94C-0AA8-BC79-D997-5964AD3FB36B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2676525" y="571500"/>
-          <a:ext cx="674224" cy="266098"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>⇒ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Fit file</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="571375" cy="266098"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{170D6686-13BF-5242-669C-17F05D1AAEB7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2676525" y="1238250"/>
-          <a:ext cx="571375" cy="266098"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="ja-JP" altLang="en-US" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>⇒ </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ja-JP" sz="1100">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Tool</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>295742</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>152747</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42CA4FE9-8671-EC29-EF42-231244A49FC5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="2667000"/>
-          <a:ext cx="3343742" cy="2486372"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>591092</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>9968</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D90662B2-DED9-80E6-BD38-4D0D997612BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4286250" y="2409825"/>
-          <a:ext cx="3886742" cy="3172268"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Arrow: Right 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{648F1480-C9C4-0517-5FA9-B2B4316172AC}"/>
+        <xdr:cNvPr id="13" name="Rectangle 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EE54449-1D77-45EC-9AE7-933C90F96F5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1061,12 +946,18 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3829050" y="4371975"/>
-          <a:ext cx="333375" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightArrow">
-          <a:avLst/>
-        </a:prstGeom>
+          <a:off x="600075" y="4295775"/>
+          <a:ext cx="2762250" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -1095,69 +986,86 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>544447</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>86391</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="Picture 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4843C52-C2B9-BF1F-F744-06C88DA58DFD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="6029325"/>
-          <a:ext cx="10907647" cy="4772691"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+      <xdr:colOff>304799</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>128588</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14288</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Connector: Curved 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9649B5E-7DAF-7801-57BE-8F5063609F3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="12" idx="1"/>
+          <a:endCxn id="13" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipH="1" flipV="1">
+          <a:off x="571499" y="2843213"/>
+          <a:ext cx="28575" cy="1600200"/>
+        </a:xfrm>
+        <a:prstGeom prst="curvedConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -800000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Rectangle 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E64B640A-9FE7-47F0-90BB-E3A2667A15E1}"/>
+        <xdr:cNvPr id="16" name="Rectangle 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40BA7FF1-BFDE-4100-8849-0E0F1BF694F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1165,8 +1073,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="571500" y="2724150"/>
-          <a:ext cx="323850" cy="238125"/>
+          <a:off x="704850" y="7524750"/>
+          <a:ext cx="2266950" cy="238125"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1205,25 +1113,69 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>315560</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>67259</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4633EA61-8005-FAB6-B94D-FCB86D17157A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="11172825"/>
+          <a:ext cx="8849960" cy="4182059"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Rectangle 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EE54449-1D77-45EC-9AE7-933C90F96F5B}"/>
+        <xdr:cNvPr id="19" name="Rectangle 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026D7EFC-69E9-4067-912D-EAB893D79435}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1231,8 +1183,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="600075" y="4295775"/>
-          <a:ext cx="2762250" cy="295275"/>
+          <a:off x="8086725" y="11515725"/>
+          <a:ext cx="247650" cy="276225"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1273,99 +1225,37 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>128588</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>14288</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connector: Curved 14">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9649B5E-7DAF-7801-57BE-8F5063609F3C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="1"/>
-          <a:endCxn id="13" idx="1"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipH="1" flipV="1">
-          <a:off x="571499" y="2843213"/>
-          <a:ext cx="28575" cy="1600200"/>
-        </a:xfrm>
-        <a:prstGeom prst="curvedConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val -800000"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Rectangle 15">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40BA7FF1-BFDE-4100-8849-0E0F1BF694F8}"/>
+        <xdr:cNvPr id="20" name="Arrow: Up 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E92EAA0-B1BB-C119-687D-30B753892BF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm>
-          <a:off x="704850" y="7524750"/>
-          <a:ext cx="2266950" cy="238125"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
+        <a:xfrm rot="20453973">
+          <a:off x="2657475" y="7762874"/>
+          <a:ext cx="171450" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="upArrow">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
           <a:solidFill>
             <a:srgbClr val="FF0000"/>
           </a:solidFill>
@@ -1398,186 +1288,11 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>315560</xdr:colOff>
-      <xdr:row>80</xdr:row>
-      <xdr:rowOff>67259</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Picture 17">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4633EA61-8005-FAB6-B94D-FCB86D17157A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="11172825"/>
-          <a:ext cx="8849960" cy="4182059"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>60</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="Rectangle 18">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{026D7EFC-69E9-4067-912D-EAB893D79435}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8086725" y="11515725"/>
-          <a:ext cx="247650" cy="276225"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="Arrow: Up 19">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E92EAA0-B1BB-C119-687D-30B753892BF9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="20453973">
-          <a:off x="2657475" y="7762874"/>
-          <a:ext cx="171450" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="upArrow">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="FF0000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="15000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="882229" cy="264560"/>
@@ -1652,13 +1367,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1717,7 +1432,7 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="470578" cy="264560"/>
@@ -1775,61 +1490,17 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114826</xdr:colOff>
-      <xdr:row>98</xdr:row>
-      <xdr:rowOff>66858</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="25" name="Picture 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26032977-FB2B-2E07-C7A3-1C81548C1A40}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="266700" y="15754350"/>
-          <a:ext cx="3772426" cy="1314633"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1845,7 +1516,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="3876675" y="16459200"/>
+          <a:off x="4610100" y="16268700"/>
           <a:ext cx="171450" cy="304800"/>
         </a:xfrm>
         <a:prstGeom prst="upArrow">
@@ -1886,12 +1557,12 @@
   </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>95</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="3014095" cy="264560"/>
+    <xdr:ext cx="1601400" cy="264560"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="27" name="TextBox 26">
@@ -1905,8 +1576,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4143375" y="16468725"/>
-          <a:ext cx="3014095" cy="264560"/>
+          <a:off x="4876800" y="16278225"/>
+          <a:ext cx="1601400" cy="264560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1939,7 +1610,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Fill target fit file</a:t>
+            <a:t>Browse target fit file</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -1947,7 +1618,7 @@
                 <a:srgbClr val="FF0000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> path **with  file name extension**</a:t>
+            <a:t> path</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1958,13 +1629,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>110</xdr:row>
+      <xdr:row>100</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>142876</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2024,13 +1695,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>125</xdr:row>
+      <xdr:row>115</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>181426</xdr:colOff>
-      <xdr:row>132</xdr:row>
+      <xdr:row>122</xdr:row>
       <xdr:rowOff>19219</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2039,6 +1710,50 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C24E1C-5180-BCC2-B932-CA2821230A5D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="24003000"/>
+          <a:ext cx="3229426" cy="1209844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>71435</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247940</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>109726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="Picture 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A12282-E09B-CC60-D605-E77B9ADB70BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2054,50 +1769,6 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="24003000"/>
-          <a:ext cx="3229426" cy="1209844"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>71435</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>247940</xdr:colOff>
-      <xdr:row>146</xdr:row>
-      <xdr:rowOff>109726</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="38" name="Picture 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30A12282-E09B-CC60-D605-E77B9ADB70BF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="3314700" y="27741560"/>
           <a:ext cx="2076740" cy="1371791"/>
         </a:xfrm>
@@ -2117,13 +1788,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>138</xdr:row>
+      <xdr:row>128</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2183,13 +1854,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>142</xdr:row>
+      <xdr:row>132</xdr:row>
       <xdr:rowOff>185831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2242,13 +1913,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>139</xdr:row>
+      <xdr:row>129</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2308,13 +1979,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>166777</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>140</xdr:row>
+      <xdr:row>130</xdr:row>
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2368,13 +2039,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>143</xdr:row>
+      <xdr:row>133</xdr:row>
       <xdr:rowOff>133351</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2434,13 +2105,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>19051</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>146</xdr:row>
+      <xdr:row>136</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2500,13 +2171,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>33909</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>144</xdr:row>
+      <xdr:row>134</xdr:row>
       <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2560,13 +2231,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>145</xdr:row>
+      <xdr:row>135</xdr:row>
       <xdr:rowOff>123826</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>38304</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>138</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2620,13 +2291,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>400051</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>161926</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>533401</xdr:colOff>
-      <xdr:row>137</xdr:row>
+      <xdr:row>127</xdr:row>
       <xdr:rowOff>104776</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2711,7 +2382,7 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1733792" cy="1124107"/>
@@ -2721,6 +2392,45 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3805CF2-9E50-4B21-9E1D-FDB7EAB6B0EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2705100" y="25003125"/>
+          <a:ext cx="1733792" cy="1124107"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1981477" cy="1124107"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ECE067-1CE8-4876-8283-1FA4E281EFB6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2736,8 +2446,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2705100" y="25003125"/>
-          <a:ext cx="1733792" cy="1124107"/>
+          <a:off x="5143500" y="25003125"/>
+          <a:ext cx="1981477" cy="1124107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2746,20 +2456,25 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1981477" cy="1124107"/>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514592</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>171607</xdr:rowOff>
+    </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9ECE067-1CE8-4876-8283-1FA4E281EFB6}"/>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7ED2A0-AA36-AE2B-1E8F-A6BE8CEEA72A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2775,8 +2490,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5143500" y="25003125"/>
-          <a:ext cx="1981477" cy="1124107"/>
+          <a:off x="266700" y="13954125"/>
+          <a:ext cx="1733792" cy="1124107"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2784,26 +2499,26 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>514592</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>171607</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102348</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>222089</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>70866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Picture 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC7ED2A0-AA36-AE2B-1E8F-A6BE8CEEA72A}"/>
+        <xdr:cNvPr id="45" name="Picture 44">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E3494D8-2F4E-AFE6-2A30-6AE99C8B15E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2819,8 +2534,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="266700" y="15859125"/>
-          <a:ext cx="1733792" cy="1124107"/>
+          <a:off x="5245848" y="19383375"/>
+          <a:ext cx="4386941" cy="3785616"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2831,23 +2546,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>102348</xdr:colOff>
-      <xdr:row>102</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209551</xdr:colOff>
+      <xdr:row>92</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>222089</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>329292</xdr:colOff>
+      <xdr:row>112</xdr:row>
       <xdr:rowOff>70866</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E3494D8-2F4E-AFE6-2A30-6AE99C8B15E6}"/>
+        <xdr:cNvPr id="46" name="Picture 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4D728B-554B-0458-41F1-CA0E38277F8D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2863,50 +2578,6 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5245848" y="19383375"/>
-          <a:ext cx="4386941" cy="3785616"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
-      <xdr:row>102</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>329292</xdr:colOff>
-      <xdr:row>122</xdr:row>
-      <xdr:rowOff>70866</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9F4D728B-554B-0458-41F1-CA0E38277F8D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="10229851" y="19383375"/>
           <a:ext cx="4386941" cy="3785616"/>
         </a:xfrm>
@@ -2921,13 +2592,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>246729</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>154496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>580104</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>11621</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2981,13 +2652,13 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>353933</xdr:colOff>
-      <xdr:row>111</xdr:row>
+      <xdr:row>101</xdr:row>
       <xdr:rowOff>154496</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>77708</xdr:colOff>
-      <xdr:row>113</xdr:row>
+      <xdr:row>103</xdr:row>
       <xdr:rowOff>11621</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3041,13 +2712,13 @@
     <xdr:from>
       <xdr:col>22</xdr:col>
       <xdr:colOff>523876</xdr:colOff>
-      <xdr:row>118</xdr:row>
+      <xdr:row>108</xdr:row>
       <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>219076</xdr:colOff>
-      <xdr:row>121</xdr:row>
+      <xdr:row>111</xdr:row>
       <xdr:rowOff>9526</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3119,7 +2790,7 @@
     <xdr:from>
       <xdr:col>17</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>101</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4283480" cy="264560"/>
@@ -3181,13 +2852,13 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>134</xdr:row>
+      <xdr:row>124</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>524342</xdr:colOff>
-      <xdr:row>141</xdr:row>
+      <xdr:row>131</xdr:row>
       <xdr:rowOff>47804</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3196,6 +2867,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C407BF7B-B12F-94B7-5C1F-CB743249D1C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5981700" y="25669875"/>
+          <a:ext cx="3343742" cy="1286054"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>453202</xdr:colOff>
+      <xdr:row>142</xdr:row>
+      <xdr:rowOff>96393</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED12F2A-AC04-60AB-065F-442A35C8B425}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3211,8 +2931,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5981700" y="25669875"/>
-          <a:ext cx="3343742" cy="1286054"/>
+          <a:off x="9810750" y="25927050"/>
+          <a:ext cx="3101152" cy="3172968"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3228,23 +2948,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>135</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>453202</xdr:colOff>
-      <xdr:row>152</xdr:row>
-      <xdr:rowOff>96393</xdr:rowOff>
+      <xdr:colOff>200433</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>67818</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="59" name="Picture 58">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1ED12F2A-AC04-60AB-065F-442A35C8B425}"/>
+        <xdr:cNvPr id="61" name="Picture 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE762BC-479B-EA7D-B342-752A5E1844F4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3254,55 +2974,6 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9810750" y="25927050"/>
-          <a:ext cx="3101152" cy="3172968"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:solidFill>
-            <a:sysClr val="windowText" lastClr="000000"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>148</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>200433</xdr:colOff>
-      <xdr:row>161</xdr:row>
-      <xdr:rowOff>67818</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Picture 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACE762BC-479B-EA7D-B342-752A5E1844F4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3660,25 +3331,25 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -3703,7 +3374,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B5091E-4ABE-4EB2-95DD-AC45409874BA}">
-  <dimension ref="A1:B134"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3725,57 +3396,62 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48">
         <v>3</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B48" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
         <v>4</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>5</v>
+      </c>
+      <c r="B81" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>6</v>
+      </c>
+      <c r="B90" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>5</v>
-      </c>
-      <c r="B82" t="s">
-        <v>10</v>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91">
-        <v>6</v>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>7</v>
       </c>
-      <c r="B91" t="s">
-        <v>8</v>
+      <c r="B114" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100">
-        <v>7</v>
-      </c>
-      <c r="B100" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -3783,24 +3459,250 @@
         <v>8</v>
       </c>
       <c r="B124" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B125" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134">
-        <v>9</v>
-      </c>
-      <c r="B134" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9D81ADBCFEAFC468F4E6027A3ED7A02" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="169b4c7a07253312a365711b40a6028d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6f212d2d-2e5c-49ac-9c61-6c58f2e79928" xmlns:ns3="498b2416-9ff5-41da-986f-a41a8a7e95e8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e51edc28a966d94cadd46e257cf24c2b" ns2:_="" ns3:_="">
+    <xsd:import namespace="6f212d2d-2e5c-49ac-9c61-6c58f2e79928"/>
+    <xsd:import namespace="498b2416-9ff5-41da-986f-a41a8a7e95e8"/>
+    <xsd:element name="properties">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element name="documentManagement">
+            <xsd:complexType>
+              <xsd:all>
+                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
+                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+              </xsd:all>
+            </xsd:complexType>
+          </xsd:element>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="6f212d2d-2e5c-49ac-9c61-6c58f2e79928" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="10" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="11" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="12" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="13" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="14" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="15" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="17" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="8cb263b1-1521-4b28-8446-98075ae54a97" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="19" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="20" nillable="true" ma:displayName="Location" ma:description="" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="498b2416-9ff5-41da-986f-a41a8a7e95e8" elementFormDefault="qualified">
+    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <xsd:element name="TaxCatchAll" ma:index="18" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{b89382c3-ec51-4656-b4c7-7cd682147e77}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="498b2416-9ff5-41da-986f-a41a8a7e95e8">
+      <xsd:complexType>
+        <xsd:complexContent>
+          <xsd:extension base="dms:MultiChoiceLookup">
+            <xsd:sequence>
+              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
+            </xsd:sequence>
+          </xsd:extension>
+        </xsd:complexContent>
+      </xsd:complexType>
+    </xsd:element>
+  </xsd:schema>
+  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
+    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
+    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
+    <xsd:element name="coreProperties" type="CT_coreProperties"/>
+    <xsd:complexType name="CT_coreProperties">
+      <xsd:all>
+        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
+        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
+          <xsd:annotation>
+            <xsd:documentation>
+                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
+                    </xsd:documentation>
+          </xsd:annotation>
+        </xsd:element>
+        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
+        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
+      </xsd:all>
+    </xsd:complexType>
+  </xsd:schema>
+  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
+    <xs:element name="Person">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:DisplayName" minOccurs="0"/>
+          <xs:element ref="pc:AccountId" minOccurs="0"/>
+          <xs:element ref="pc:AccountType" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="DisplayName" type="xs:string"/>
+    <xs:element name="AccountId" type="xs:string"/>
+    <xs:element name="AccountType" type="xs:string"/>
+    <xs:element name="BDCAssociatedEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+        <xs:attribute ref="pc:EntityNamespace"/>
+        <xs:attribute ref="pc:EntityName"/>
+        <xs:attribute ref="pc:SystemInstanceName"/>
+        <xs:attribute ref="pc:AssociationName"/>
+      </xs:complexType>
+    </xs:element>
+    <xs:attribute name="EntityNamespace" type="xs:string"/>
+    <xs:attribute name="EntityName" type="xs:string"/>
+    <xs:attribute name="SystemInstanceName" type="xs:string"/>
+    <xs:attribute name="AssociationName" type="xs:string"/>
+    <xs:element name="BDCEntity">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
+          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
+          <xs:element ref="pc:EntityId1" minOccurs="0"/>
+          <xs:element ref="pc:EntityId2" minOccurs="0"/>
+          <xs:element ref="pc:EntityId3" minOccurs="0"/>
+          <xs:element ref="pc:EntityId4" minOccurs="0"/>
+          <xs:element ref="pc:EntityId5" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="EntityDisplayName" type="xs:string"/>
+    <xs:element name="EntityInstanceReference" type="xs:string"/>
+    <xs:element name="EntityId1" type="xs:string"/>
+    <xs:element name="EntityId2" type="xs:string"/>
+    <xs:element name="EntityId3" type="xs:string"/>
+    <xs:element name="EntityId4" type="xs:string"/>
+    <xs:element name="EntityId5" type="xs:string"/>
+    <xs:element name="Terms">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermInfo">
+      <xs:complexType>
+        <xs:sequence>
+          <xs:element ref="pc:TermName" minOccurs="0"/>
+          <xs:element ref="pc:TermId" minOccurs="0"/>
+        </xs:sequence>
+      </xs:complexType>
+    </xs:element>
+    <xs:element name="TermName" type="xs:string"/>
+    <xs:element name="TermId" type="xs:string"/>
+  </xs:schema>
+</ct:contentTypeSchema>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="6f212d2d-2e5c-49ac-9c61-6c58f2e79928">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="498b2416-9ff5-41da-986f-a41a8a7e95e8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6F660B60-4702-4DB8-810B-9200800A0B9C}"/>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F5E4975-DFD2-4102-94B5-8D685AACC1B4}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9DF79FF-9565-4C90-875C-4BD4F214AFA4}"/>
 </file>
</xml_diff>